<commit_message>
sends email to customer with results file
</commit_message>
<xml_diff>
--- a/P2_Performer/Results/03-27-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
+++ b/P2_Performer/Results/03-27-2023/Rich Drexel - Dallas, Texas, United States of America.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Revature\GetawayGurus\P2_Performer\Results\03-27-2023\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B33A93BB-F6D9-461B-A922-95127A6BB00A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{CC7DB28A-162C-430C-A2D2-A53E15EEC57C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2004" yWindow="2364" windowWidth="17280" windowHeight="8964" xr2:uid="{A1FAF4A7-F0BB-4497-A1BA-7F4F59656CDF}"/>
   </bookViews>
@@ -47,9 +47,6 @@
     <t># of Nights</t>
   </si>
   <si>
-    <t>Total</t>
-  </si>
-  <si>
     <t>Max Temp</t>
   </si>
   <si>
@@ -74,6 +71,9 @@
     <t>Restaurant</t>
   </si>
   <si>
+    <t>Total Per Room</t>
+  </si>
+  <si>
     <t>Majestic Theatre</t>
   </si>
   <si>
@@ -131,7 +131,7 @@
     <t>Omni Dallas Hotel</t>
   </si>
   <si>
-    <t>The Westin Dallas Park Central</t>
+    <t>DoubleTree by Hilton Dallas Near the Galleria</t>
   </si>
   <si>
     <t>Hilton Dallas/Park Cities</t>
@@ -734,17 +734,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="38" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="39" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -754,6 +749,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -773,13 +771,15 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="32" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="19" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="2" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="14" fontId="2" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="2" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1097,12 +1097,12 @@
   <dimension ref="A1:E31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="28.77734375" customWidth="1"/>
+    <col min="1" max="1" width="32.33203125" customWidth="1"/>
     <col min="2" max="4" width="11.77734375" customWidth="1"/>
     <col min="5" max="5" width="31.44140625" customWidth="1"/>
   </cols>
@@ -1117,343 +1117,323 @@
       <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="38" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="39"/>
+      <c r="D1" s="36" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" s="37"/>
     </row>
     <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="10" t="s">
         <v>30</v>
       </c>
-      <c r="B2" s="47">
-        <v>172</v>
+      <c r="B2" s="48">
+        <v>274</v>
       </c>
       <c r="C2" s="11">
-        <v>8</v>
-      </c>
-      <c r="D2" s="40">
+        <v>6</v>
+      </c>
+      <c r="D2" s="38">
         <f>PRODUCT(B2,C2)</f>
-        <v>1376</v>
-      </c>
-      <c r="E2" s="41"/>
+        <v>1644</v>
+      </c>
+      <c r="E2" s="39"/>
     </row>
     <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="B3" s="48">
-        <v>149</v>
+      <c r="B3" s="49">
+        <v>159</v>
       </c>
       <c r="C3" s="8">
-        <v>8</v>
-      </c>
-      <c r="D3" s="40">
+        <v>6</v>
+      </c>
+      <c r="D3" s="38">
         <f t="shared" ref="D3:D4" si="0">PRODUCT(B3,C3)</f>
-        <v>1192</v>
-      </c>
-      <c r="E3" s="41"/>
+        <v>954</v>
+      </c>
+      <c r="E3" s="39"/>
     </row>
     <row r="4" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A4" s="12" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="49">
+      <c r="B4" s="50">
         <v>295</v>
       </c>
       <c r="C4" s="13">
-        <v>8</v>
-      </c>
-      <c r="D4" s="40">
+        <v>6</v>
+      </c>
+      <c r="D4" s="38">
         <f t="shared" si="0"/>
-        <v>2360</v>
-      </c>
-      <c r="E4" s="41"/>
+        <v>1770</v>
+      </c>
+      <c r="E4" s="39"/>
     </row>
     <row r="5" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="40" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="42" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="43"/>
+      <c r="C5" s="40"/>
+      <c r="D5" s="40"/>
+      <c r="E5" s="41"/>
     </row>
     <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="44" t="s">
+      <c r="B6" s="42" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="46"/>
+      <c r="C6" s="43"/>
+      <c r="D6" s="43"/>
+      <c r="E6" s="44"/>
     </row>
     <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="30" t="s">
+      <c r="B7" s="31" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="31"/>
-      <c r="D7" s="31"/>
-      <c r="E7" s="32"/>
+      <c r="C7" s="32"/>
+      <c r="D7" s="32"/>
+      <c r="E7" s="33"/>
     </row>
     <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="B8" s="30" t="s">
+      <c r="B8" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="C8" s="31"/>
-      <c r="D8" s="31"/>
-      <c r="E8" s="32"/>
+      <c r="C8" s="32"/>
+      <c r="D8" s="32"/>
+      <c r="E8" s="33"/>
     </row>
     <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="B9" s="30" t="s">
+      <c r="B9" s="31" t="s">
         <v>19</v>
       </c>
-      <c r="C9" s="31"/>
-      <c r="D9" s="31"/>
-      <c r="E9" s="32"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="32"/>
+      <c r="E9" s="33"/>
     </row>
     <row r="10" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A10" s="12" t="s">
         <v>20</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="C10" s="36"/>
-      <c r="D10" s="36"/>
-      <c r="E10" s="37"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="35"/>
     </row>
     <row r="11" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="B11" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="C11" s="34"/>
-      <c r="D11" s="34"/>
-      <c r="E11" s="35"/>
+      <c r="B11" s="28" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="29"/>
+      <c r="D11" s="29"/>
+      <c r="E11" s="30"/>
     </row>
     <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A12" s="10" t="s">
         <v>22</v>
       </c>
-      <c r="B12" s="27" t="s">
+      <c r="B12" s="45" t="s">
         <v>23</v>
       </c>
-      <c r="C12" s="28"/>
-      <c r="D12" s="28"/>
-      <c r="E12" s="29"/>
+      <c r="C12" s="46"/>
+      <c r="D12" s="46"/>
+      <c r="E12" s="47"/>
     </row>
     <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A13" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="31" t="s">
         <v>13</v>
       </c>
-      <c r="C13" s="31"/>
-      <c r="D13" s="31"/>
-      <c r="E13" s="32"/>
+      <c r="C13" s="32"/>
+      <c r="D13" s="32"/>
+      <c r="E13" s="33"/>
     </row>
     <row r="14" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A14" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="B14" s="30" t="s">
+      <c r="B14" s="31" t="s">
         <v>25</v>
       </c>
-      <c r="C14" s="31"/>
-      <c r="D14" s="31"/>
-      <c r="E14" s="32"/>
+      <c r="C14" s="32"/>
+      <c r="D14" s="32"/>
+      <c r="E14" s="33"/>
     </row>
     <row r="15" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A15" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="30" t="s">
+      <c r="B15" s="31" t="s">
         <v>27</v>
       </c>
-      <c r="C15" s="31"/>
-      <c r="D15" s="31"/>
-      <c r="E15" s="32"/>
+      <c r="C15" s="32"/>
+      <c r="D15" s="32"/>
+      <c r="E15" s="33"/>
     </row>
     <row r="16" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A16" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="B16" s="30" t="s">
+      <c r="B16" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="31"/>
-      <c r="D16" s="31"/>
-      <c r="E16" s="32"/>
+      <c r="C16" s="32"/>
+      <c r="D16" s="32"/>
+      <c r="E16" s="33"/>
     </row>
     <row r="17" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A17" s="14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="15" t="s">
         <v>7</v>
       </c>
-      <c r="B17" s="15" t="s">
-        <v>8</v>
-      </c>
       <c r="C17" s="16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" s="17" t="s">
         <v>4</v>
       </c>
-      <c r="D17" s="17" t="s">
+      <c r="E17" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="E17" s="18" t="s">
-        <v>6</v>
-      </c>
     </row>
     <row r="18" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A18" s="50">
-        <v>45037</v>
+      <c r="A18" s="51">
+        <v>45039</v>
       </c>
       <c r="B18" s="19">
-        <v>56.5</v>
-      </c>
-      <c r="C18" s="22">
-        <v>75.7</v>
+        <v>59.6</v>
+      </c>
+      <c r="C18" s="23">
+        <v>77.599999999999994</v>
       </c>
       <c r="D18" s="19">
-        <v>12.8</v>
-      </c>
-      <c r="E18" s="23">
+        <v>13.9</v>
+      </c>
+      <c r="E18" s="24">
+        <v>0.15</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A19" s="52">
+        <v>45040</v>
+      </c>
+      <c r="B19" s="8">
+        <v>59.4</v>
+      </c>
+      <c r="C19" s="8">
+        <v>76.400000000000006</v>
+      </c>
+      <c r="D19" s="7">
+        <v>15.4</v>
+      </c>
+      <c r="E19" s="9">
+        <v>0.45</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A20" s="52">
+        <v>45041</v>
+      </c>
+      <c r="B20" s="8">
+        <v>59.1</v>
+      </c>
+      <c r="C20" s="8">
+        <v>78.2</v>
+      </c>
+      <c r="D20" s="7">
+        <v>14.6</v>
+      </c>
+      <c r="E20" s="9">
+        <v>0.11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A21" s="52">
+        <v>45042</v>
+      </c>
+      <c r="B21" s="8">
+        <v>60.3</v>
+      </c>
+      <c r="C21" s="8">
+        <v>77.900000000000006</v>
+      </c>
+      <c r="D21" s="7">
+        <v>14</v>
+      </c>
+      <c r="E21" s="9">
+        <v>0.12</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A22" s="52">
+        <v>45043</v>
+      </c>
+      <c r="B22" s="8">
+        <v>60.2</v>
+      </c>
+      <c r="C22" s="8">
+        <v>76.900000000000006</v>
+      </c>
+      <c r="D22" s="7">
+        <v>14.7</v>
+      </c>
+      <c r="E22" s="9">
+        <v>0.26</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A23" s="53">
+        <v>45044</v>
+      </c>
+      <c r="B23" s="5">
+        <v>60.6</v>
+      </c>
+      <c r="C23" s="5">
+        <v>80.7</v>
+      </c>
+      <c r="D23" s="5">
+        <v>13.1</v>
+      </c>
+      <c r="E23" s="9">
         <v>0.13</v>
       </c>
     </row>
-    <row r="19" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="51">
-        <v>45038</v>
-      </c>
-      <c r="B19" s="8">
-        <v>59.1</v>
-      </c>
-      <c r="C19" s="8">
-        <v>76.900000000000006</v>
-      </c>
-      <c r="D19" s="7">
-        <v>14.6</v>
-      </c>
-      <c r="E19" s="9">
-        <v>0.03</v>
-      </c>
-    </row>
-    <row r="20" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="51">
-        <v>45039</v>
-      </c>
-      <c r="B20" s="8">
-        <v>59.6</v>
-      </c>
-      <c r="C20" s="8">
-        <v>77.599999999999994</v>
-      </c>
-      <c r="D20" s="7">
-        <v>13.9</v>
-      </c>
-      <c r="E20" s="9">
-        <v>0.15</v>
-      </c>
-    </row>
-    <row r="21" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="51">
-        <v>45040</v>
-      </c>
-      <c r="B21" s="8">
-        <v>59.4</v>
-      </c>
-      <c r="C21" s="8">
-        <v>76.400000000000006</v>
-      </c>
-      <c r="D21" s="7">
-        <v>15.4</v>
-      </c>
-      <c r="E21" s="9">
-        <v>0.45</v>
-      </c>
-    </row>
-    <row r="22" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="51">
-        <v>45041</v>
-      </c>
-      <c r="B22" s="8">
-        <v>59.1</v>
-      </c>
-      <c r="C22" s="8">
-        <v>78.2</v>
-      </c>
-      <c r="D22" s="7">
-        <v>14.6</v>
-      </c>
-      <c r="E22" s="9">
-        <v>0.11</v>
-      </c>
-    </row>
-    <row r="23" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="52">
-        <v>45042</v>
-      </c>
-      <c r="B23" s="5">
-        <v>60.3</v>
-      </c>
-      <c r="C23" s="5">
-        <v>77.900000000000006</v>
-      </c>
-      <c r="D23" s="5">
-        <v>14</v>
-      </c>
-      <c r="E23" s="9">
-        <v>0.12</v>
-      </c>
-    </row>
     <row r="24" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="53">
-        <v>45043</v>
-      </c>
-      <c r="B24" s="21">
-        <v>60.2</v>
-      </c>
-      <c r="C24" s="21">
-        <v>76.900000000000006</v>
-      </c>
-      <c r="D24" s="21">
-        <v>14.7</v>
-      </c>
-      <c r="E24" s="20">
-        <v>0.26</v>
-      </c>
+      <c r="A24" s="22"/>
+      <c r="B24" s="21"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="21"/>
+      <c r="E24" s="20"/>
     </row>
     <row r="25" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A25" s="51">
-        <v>45044</v>
-      </c>
-      <c r="B25" s="8">
-        <v>60.6</v>
-      </c>
-      <c r="C25" s="8">
-        <v>80.7</v>
-      </c>
-      <c r="D25" s="8">
-        <v>13.1</v>
-      </c>
-      <c r="E25" s="9">
-        <v>0.13</v>
-      </c>
+      <c r="A25" s="6"/>
+      <c r="B25" s="8"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="9"/>
     </row>
     <row r="26" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A26" s="6"/>
@@ -1491,14 +1471,19 @@
       <c r="E30" s="9"/>
     </row>
     <row r="31" spans="1:5" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A31" s="24"/>
-      <c r="B31" s="25"/>
-      <c r="C31" s="25"/>
-      <c r="D31" s="25"/>
-      <c r="E31" s="26"/>
+      <c r="A31" s="25"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="27"/>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="B12:E12"/>
+    <mergeCell ref="B13:E13"/>
+    <mergeCell ref="B14:E14"/>
+    <mergeCell ref="B15:E15"/>
+    <mergeCell ref="B16:E16"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B9:E9"/>
     <mergeCell ref="B10:E10"/>
@@ -1510,11 +1495,6 @@
     <mergeCell ref="B8:E8"/>
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="D4:E4"/>
-    <mergeCell ref="B12:E12"/>
-    <mergeCell ref="B13:E13"/>
-    <mergeCell ref="B14:E14"/>
-    <mergeCell ref="B15:E15"/>
-    <mergeCell ref="B16:E16"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>